<commit_message>
excel changed by abhishek
</commit_message>
<xml_diff>
--- a/Std1A.xlsx
+++ b/Std1A.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myshala\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\abhishek\myshala\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
   <si>
     <t>RollNo</t>
   </si>
@@ -45,6 +45,15 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>dss</t>
   </si>
 </sst>
 </file>
@@ -374,7 +383,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,6 +415,9 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
       <c r="G2" s="1">
         <f>SUM(D2:F2)</f>
         <v>0</v>
@@ -415,6 +427,9 @@
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
       <c r="G3" s="1">
         <f t="shared" ref="G3:G20" si="0">SUM(D3:F3)</f>
         <v>0</v>
@@ -424,6 +439,9 @@
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -433,6 +451,9 @@
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -442,6 +463,9 @@
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -451,6 +475,9 @@
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -458,6 +485,9 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
         <v>7</v>
       </c>
       <c r="G8" s="1">
@@ -469,6 +499,9 @@
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -478,6 +511,9 @@
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -487,6 +523,9 @@
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
       <c r="G11" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -496,6 +535,9 @@
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
       <c r="G12" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -505,6 +547,9 @@
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
       <c r="G13" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -514,6 +559,9 @@
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
       <c r="G14" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -523,6 +571,9 @@
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
       <c r="G15" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -532,6 +583,9 @@
       <c r="A16">
         <v>15</v>
       </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
       <c r="G16" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -541,6 +595,9 @@
       <c r="A17">
         <v>16</v>
       </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
       <c r="G17" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -550,6 +607,9 @@
       <c r="A18">
         <v>17</v>
       </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
       <c r="G18" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -559,6 +619,9 @@
       <c r="A19">
         <v>18</v>
       </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
       <c r="G19" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -567,6 +630,9 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
entered eng & maths marks
</commit_message>
<xml_diff>
--- a/Std1A.xlsx
+++ b/Std1A.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\abhishek\myshala\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vinod\myshala\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="14">
   <si>
     <t>RollNo</t>
   </si>
@@ -54,6 +54,18 @@
   </si>
   <si>
     <t>dss</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -383,7 +395,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,221 +427,386 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
       <c r="C2" t="s">
         <v>7</v>
+      </c>
+      <c r="D2">
+        <v>45</v>
+      </c>
+      <c r="E2">
+        <v>45</v>
       </c>
       <c r="G2" s="1">
         <f>SUM(D2:F2)</f>
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
       <c r="C3" t="s">
         <v>7</v>
+      </c>
+      <c r="D3">
+        <v>32</v>
+      </c>
+      <c r="E3">
+        <v>32</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" ref="G3:G20" si="0">SUM(D3:F3)</f>
-        <v>0</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
+      <c r="D4">
+        <v>45</v>
+      </c>
+      <c r="E4">
+        <v>45</v>
+      </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
+      <c r="D5">
+        <v>45</v>
+      </c>
+      <c r="E5">
+        <v>45</v>
+      </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>9</v>
+      </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
+      <c r="D8">
+        <v>36</v>
+      </c>
+      <c r="E8">
+        <v>36</v>
+      </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
       <c r="C9" t="s">
         <v>9</v>
       </c>
+      <c r="D9">
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <v>14</v>
+      </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
+      <c r="D10">
+        <v>48</v>
+      </c>
+      <c r="E10">
+        <v>48</v>
+      </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
+      <c r="D11">
+        <v>42</v>
+      </c>
+      <c r="E11">
+        <v>42</v>
+      </c>
       <c r="G11" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
+      <c r="D12">
+        <v>36</v>
+      </c>
+      <c r="E12">
+        <v>36</v>
+      </c>
       <c r="G12" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
+      <c r="D13">
+        <v>38</v>
+      </c>
+      <c r="E13">
+        <v>38</v>
+      </c>
       <c r="G13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
       <c r="C14" t="s">
         <v>9</v>
       </c>
+      <c r="D14">
+        <v>7</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
+      </c>
       <c r="G14" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
+      <c r="D15">
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <v>9</v>
+      </c>
       <c r="G15" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
+      <c r="D16">
+        <v>36</v>
+      </c>
+      <c r="E16">
+        <v>36</v>
+      </c>
       <c r="G16" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
+      <c r="D17">
+        <v>14</v>
+      </c>
+      <c r="E17">
+        <v>14</v>
+      </c>
       <c r="G17" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
       <c r="C18" t="s">
         <v>7</v>
       </c>
+      <c r="D18">
+        <v>48</v>
+      </c>
+      <c r="E18">
+        <v>48</v>
+      </c>
       <c r="G18" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
       <c r="C19" t="s">
         <v>7</v>
       </c>
+      <c r="D19">
+        <v>42</v>
+      </c>
+      <c r="E19">
+        <v>42</v>
+      </c>
       <c r="G19" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
avg added to std 1A.xlsx
</commit_message>
<xml_diff>
--- a/Std1A.xlsx
+++ b/Std1A.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SachinTanpure\myshala\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vinod\myshala\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="17">
   <si>
     <t>RollNo</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Sachin</t>
+  </si>
+  <si>
+    <t>Avarage</t>
   </si>
 </sst>
 </file>
@@ -393,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,7 +407,7 @@
     <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,8 +429,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -450,8 +456,12 @@
         <f t="shared" ref="G2:G20" si="0">SUM(D2:F2)</f>
         <v>110</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f>AVERAGE(D2:F2)</f>
+        <v>36.666666666666664</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -474,8 +484,12 @@
         <f t="shared" si="0"/>
         <v>108</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f t="shared" ref="H3:H23" si="1">AVERAGE(D3:F3)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -498,8 +512,12 @@
         <f t="shared" si="0"/>
         <v>113</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>37.666666666666664</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -522,8 +540,12 @@
         <f t="shared" si="0"/>
         <v>146</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>48.666666666666664</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -546,8 +568,12 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>14.666666666666666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -570,8 +596,12 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -594,8 +624,12 @@
         <f t="shared" si="0"/>
         <v>130</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>43.333333333333336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -618,8 +652,12 @@
         <f t="shared" si="0"/>
         <v>124</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>41.333333333333336</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -642,8 +680,12 @@
         <f t="shared" si="0"/>
         <v>148</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>49.333333333333336</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -666,8 +708,12 @@
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -690,8 +736,12 @@
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>24.333333333333332</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -714,8 +764,12 @@
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>26.333333333333332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -738,8 +792,12 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>6.333333333333333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -762,8 +820,12 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -786,8 +848,12 @@
         <f t="shared" si="0"/>
         <v>127</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>42.333333333333336</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -810,8 +876,12 @@
         <f t="shared" si="0"/>
         <v>116</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>38.666666666666664</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -834,8 +904,12 @@
         <f t="shared" si="0"/>
         <v>186</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -858,8 +932,12 @@
         <f t="shared" si="0"/>
         <v>126</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -882,8 +960,12 @@
         <f t="shared" si="0"/>
         <v>81</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -905,8 +987,12 @@
       <c r="G21">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -928,8 +1014,12 @@
       <c r="G22">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -950,6 +1040,10 @@
       </c>
       <c r="G23">
         <v>15</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>